<commit_message>
Added school to database
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275"/>
   </bookViews>
   <sheets>
     <sheet name="grade56" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
   <si>
     <t>6klasnici</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>Sasho</t>
+  </si>
+  <si>
+    <t>NPMG</t>
+  </si>
+  <si>
+    <t>OMG</t>
+  </si>
+  <si>
+    <t>PMG</t>
   </si>
 </sst>
 </file>
@@ -578,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,133 +598,148 @@
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -726,10 +750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,98 +761,110 @@
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>57</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>51</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>52</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>46</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>55</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -839,10 +875,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,29 +886,32 @@
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>